<commit_message>
updated challenge.xlsx to delete the space in the Last Name column
</commit_message>
<xml_diff>
--- a/src/Week 7/homework/challenge.xlsx
+++ b/src/Week 7/homework/challenge.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\UiPath\RPAChallenge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LucianaBogdan\Documents\GitHub\rpa_bootcamp_march\src\Week 7\homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DCE12F-66F4-48CA-94C4-BA0278685606}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3228" yWindow="2508" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,9 +23,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
   <si>
     <t>First Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Name </t>
   </si>
   <si>
     <t>Company Name</t>
@@ -205,6 +203,9 @@
   </si>
   <si>
     <t>lpalmer@timepath.co.uk</t>
+  </si>
+  <si>
+    <t>Last Name</t>
   </si>
 </sst>
 </file>
@@ -616,7 +617,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -637,43 +638,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G2" s="4">
         <v>40716543298</v>
@@ -682,22 +683,22 @@
     </row>
     <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3" s="4">
         <v>40791345621</v>
@@ -706,22 +707,22 @@
     </row>
     <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G4" s="4">
         <v>40735416854</v>
@@ -730,22 +731,22 @@
     </row>
     <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" s="4">
         <v>40733652145</v>
@@ -754,22 +755,22 @@
     </row>
     <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G6" s="4">
         <v>40799885412</v>
@@ -778,22 +779,22 @@
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G7" s="4">
         <v>40733154268</v>
@@ -802,22 +803,22 @@
     </row>
     <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="F8" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G8" s="4">
         <v>40712462257</v>
@@ -826,22 +827,22 @@
     </row>
     <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="F9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9" s="4">
         <v>40731254562</v>
@@ -850,22 +851,22 @@
     </row>
     <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="F10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G10" s="4">
         <v>40741785214</v>
@@ -874,22 +875,22 @@
     </row>
     <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="F11" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G11" s="4">
         <v>40731653845</v>

</xml_diff>

<commit_message>
Revert "Week 7 homework"
</commit_message>
<xml_diff>
--- a/src/Week 7/homework/challenge.xlsx
+++ b/src/Week 7/homework/challenge.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LucianaBogdan\Documents\GitHub\rpa_bootcamp_march\src\Week 7\homework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\UiPath\RPAChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DCE12F-66F4-48CA-94C4-BA0278685606}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3228" yWindow="2508" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +22,9 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
   <si>
     <t>First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Name </t>
   </si>
   <si>
     <t>Company Name</t>
@@ -203,9 +205,6 @@
   </si>
   <si>
     <t>lpalmer@timepath.co.uk</t>
-  </si>
-  <si>
-    <t>Last Name</t>
   </si>
 </sst>
 </file>
@@ -617,7 +616,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -638,43 +637,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G2" s="4">
         <v>40716543298</v>
@@ -683,22 +682,22 @@
     </row>
     <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G3" s="4">
         <v>40791345621</v>
@@ -707,22 +706,22 @@
     </row>
     <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G4" s="4">
         <v>40735416854</v>
@@ -731,22 +730,22 @@
     </row>
     <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G5" s="4">
         <v>40733652145</v>
@@ -755,22 +754,22 @@
     </row>
     <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G6" s="4">
         <v>40799885412</v>
@@ -779,22 +778,22 @@
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G7" s="4">
         <v>40733154268</v>
@@ -803,22 +802,22 @@
     </row>
     <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G8" s="4">
         <v>40712462257</v>
@@ -827,22 +826,22 @@
     </row>
     <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G9" s="4">
         <v>40731254562</v>
@@ -851,22 +850,22 @@
     </row>
     <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G10" s="4">
         <v>40741785214</v>
@@ -875,22 +874,22 @@
     </row>
     <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G11" s="4">
         <v>40731653845</v>

</xml_diff>